<commit_message>
Project 1 - code till Sep 24th
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/excels/MasterTestData.xlsx
+++ b/src/test/resources/testdata/excels/MasterTestData.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FLM2ndJuneWS\FrameworkPOM\src\test\resources\testdata\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF13C08-3AB0-4B5B-9E82-F1DE7731EE07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C960C432-617D-4099-9ED9-D46041FD77E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{01F410BB-4CDF-4E65-BF55-31489716C62E}"/>
   </bookViews>
   <sheets>
     <sheet name="regression" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
   <si>
     <t>TC101</t>
   </si>
@@ -85,6 +88,9 @@
   </si>
   <si>
     <t>India</t>
+  </si>
+  <si>
+    <t>Adactin.com - New User Registration</t>
   </si>
 </sst>
 </file>
@@ -455,25 +461,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC914BC-115C-4E99-A655-A098063134BC}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D2"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="20.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,7 +493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,56 +507,253 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1" xr:uid="{89B35990-389A-4C7A-8FC0-7A201128435F}"/>
+    <hyperlink ref="G5" r:id="rId1" xr:uid="{89B35990-389A-4C7A-8FC0-7A201128435F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF483CA1-8A81-470E-9F54-4AB4CD812302}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{DBB03F52-66A4-4A56-BBFB-6AF1FEDED046}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221370A0-2817-458E-BCED-DDDAEB7E35A3}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC191BE-5BA8-47D3-811B-69D9ACAF5400}">
+  <dimension ref="C1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:4" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="3:4" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Project 1 - code till Sep 25th
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/excels/MasterTestData.xlsx
+++ b/src/test/resources/testdata/excels/MasterTestData.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FLM2ndJuneWS\FrameworkPOM\src\test\resources\testdata\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C960C432-617D-4099-9ED9-D46041FD77E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC5B2EA-2537-4007-ABD4-67673B59F46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{01F410BB-4CDF-4E65-BF55-31489716C62E}"/>
+    <workbookView xWindow="1416" yWindow="1128" windowWidth="21624" windowHeight="11112" xr2:uid="{01F410BB-4CDF-4E65-BF55-31489716C62E}"/>
   </bookViews>
   <sheets>
     <sheet name="regression" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="smoke" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="21">
   <si>
     <t>TC101</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>Adactin.com - New User Registration</t>
+  </si>
+  <si>
+    <t>TC103</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Sydney</t>
   </si>
 </sst>
 </file>
@@ -461,16 +470,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC914BC-115C-4E99-A655-A098063134BC}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="20.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="1" bestFit="1" customWidth="1"/>
@@ -489,9 +498,6 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
@@ -503,9 +509,6 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
@@ -557,6 +560,22 @@
       </c>
       <c r="H5" s="1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -572,9 +591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF483CA1-8A81-470E-9F54-4AB4CD812302}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>